<commit_message>
added STL File and updated BOM
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/BOM_V1.0.xlsx
+++ b/Documentation/BOMs/BOM_V1.0.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Item</t>
   </si>
@@ -60,9 +60,6 @@
     <t>This is all of the bracetry and hardware for the CNC Machine</t>
   </si>
   <si>
-    <t>Limit Switches</t>
-  </si>
-  <si>
     <t xml:space="preserve">PCI I/O Card </t>
   </si>
   <si>
@@ -121,6 +118,42 @@
   </si>
   <si>
     <t>Incremental Encoder</t>
+  </si>
+  <si>
+    <t>Stepper motor for the X axis</t>
+  </si>
+  <si>
+    <t>Stepper Motor for the Y axis</t>
+  </si>
+  <si>
+    <t>Stepper Moto for the Z axis</t>
+  </si>
+  <si>
+    <t>PCI I/O Card with Digital and Analog I/O</t>
+  </si>
+  <si>
+    <t>Limit and Home Switches</t>
+  </si>
+  <si>
+    <t>Interface Card for communicating with servo motors</t>
+  </si>
+  <si>
+    <t>I/O card used for limit and home switches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp range x -x </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outputs a single Voltage</t>
+  </si>
+  <si>
+    <t>Wire Feed Welder that uses inert sheilding gas</t>
+  </si>
+  <si>
+    <t>Used for controlling the motors on the welder control knobs</t>
+  </si>
+  <si>
+    <t>Used for connecting signals to the PCIe card</t>
   </si>
 </sst>
 </file>
@@ -531,7 +564,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -539,11 +572,12 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -578,16 +612,25 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -605,10 +648,13 @@
       <c r="E9" s="1">
         <v>677</v>
       </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -616,58 +662,73 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>26</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -675,55 +736,66 @@
       <c r="C17">
         <v>5056</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>